<commit_message>
creazione della pagina di importazione della classe, correzione della pianificazione dei docenti, spostamento del sito web sul nuovo server, diari settimana 13-16.02.2017
</commit_message>
<xml_diff>
--- a/Progettazione2/Analisi/requisiti.xlsx
+++ b/Progettazione2/Analisi/requisiti.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>REQ-008 progetto precedente</t>
+  </si>
+  <si>
+    <t>discutere su cosa se si dovesse avere tempo di farlo</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C151" sqref="B2:C151"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,7 +1723,9 @@
       <c r="B149" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C149" s="3"/>
+      <c r="C149" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="150" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="1" t="s">

</xml_diff>

<commit_message>
agigunta dell'attributo pia_gruppo e modifica di tutte le pagine aggiunta pagina log e aggiustamento proposte spostamento file js
</commit_message>
<xml_diff>
--- a/Progettazione2/Analisi/requisiti.xlsx
+++ b/Progettazione2/Analisi/requisiti.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="104">
   <si>
     <t>ID</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Pagina di Log</t>
   </si>
   <si>
-    <t>Per ogni log bisogna sapere il docente che effettua l'azione, il tipo di azione, la pagina in cui avviene l'azione, un ev. descrizione e la data</t>
-  </si>
-  <si>
     <t>Prevedere una barra di ricerca o filtraggio</t>
   </si>
   <si>
@@ -309,6 +306,36 @@
   </si>
   <si>
     <t>discutere su cosa se si dovesse avere tempo di farlo</t>
+  </si>
+  <si>
+    <t>Per ogni log bisogna sapere il docente o l'email che effettua l'azione, il tipo di azione, la pagina in cui avviene l'azione, un ev. descrizione e la data</t>
+  </si>
+  <si>
+    <t>REQ-014</t>
+  </si>
+  <si>
+    <t>Pagina Visione Pianificazione Docenti MP (Responsabile)</t>
+  </si>
+  <si>
+    <t>Accessibile solo ai responsabili e all'Amministratore</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutte le informazioni delle pianificazioni</t>
+  </si>
+  <si>
+    <t>Bisogna avere una barra di ricerca per trovare le pianificazioni</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere la percentuale di lavoro dei docenti in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna avere un bottone per l'eliminazione della pianificazione tramite una conferma</t>
+  </si>
+  <si>
+    <t>Bisogna avere un bottone per vedere in dettaglio la pianificazione del docente in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna poter permettere al responsabile di modificare le ore totali in caso si avesse sbagliato nella creazione della pianificazione</t>
   </si>
 </sst>
 </file>
@@ -335,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +372,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -471,6 +504,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -753,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C151"/>
+  <dimension ref="B1:C168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,7 +841,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -840,7 +879,7 @@
     <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -849,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -881,7 +920,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -944,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -976,7 +1015,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1005,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1037,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1123,13 +1162,13 @@
     <row r="56" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
       <c r="C56" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
       <c r="C57" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1140,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1172,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1282,7 +1321,7 @@
         <v>6</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1387,7 +1426,7 @@
         <v>6</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1484,37 +1523,37 @@
     <row r="112" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="6" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="5"/>
       <c r="C113" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="5"/>
       <c r="C114" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="5"/>
       <c r="C115" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="7"/>
       <c r="C116" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="5"/>
       <c r="C117" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1531,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1567,13 +1606,13 @@
     <row r="125" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="1"/>
       <c r="C125" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="126" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
       <c r="C126" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1594,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1630,7 +1669,7 @@
     <row r="135" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="5"/>
       <c r="C135" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1639,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1647,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="139" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1683,7 +1722,7 @@
     <row r="143" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="5"/>
       <c r="C143" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1700,7 +1739,7 @@
         <v>1</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1724,7 +1763,7 @@
         <v>6</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1738,13 +1777,117 @@
     <row r="151" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="5"/>
       <c r="C151" s="6" t="s">
-        <v>74</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="153" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B156" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="5"/>
+      <c r="C159" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="5"/>
+      <c r="C160" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="5"/>
+      <c r="C161" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="5"/>
+      <c r="C162" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B163" s="5"/>
+      <c r="C163" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="7"/>
+      <c r="C164" s="22"/>
+    </row>
+    <row r="165" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="7"/>
+      <c r="C165" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B166" s="7"/>
+      <c r="C166" s="22"/>
+    </row>
+    <row r="167" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B167" s="7"/>
+      <c r="C167" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B168" s="7"/>
+      <c r="C168" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="C167:C168"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
manuale e inizio pagina approcci interdisciplinari tematici
</commit_message>
<xml_diff>
--- a/Progettazione2/Analisi/requisiti.xlsx
+++ b/Progettazione2/Analisi/requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione2\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione2\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Informazione classe</t>
   </si>
   <si>
-    <t>Bisogna poter vedere tutti i dati degli ovvero nome, data di nascita e altre informazioni</t>
-  </si>
-  <si>
     <t>la pagina è accessibile solo all'A</t>
   </si>
   <si>
@@ -336,6 +333,39 @@
   </si>
   <si>
     <t>Bisogna poter permettere al responsabile di modificare le ore totali in caso si avesse sbagliato nella creazione della pianificazione</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>REQ-015</t>
+  </si>
+  <si>
+    <t>Pagina Pianificazione Docenti MP</t>
+  </si>
+  <si>
+    <t>Accessibile solo al Responsabile e all'Amministratore</t>
+  </si>
+  <si>
+    <t>Bisogna pianificare un minimo di 2 docenti</t>
+  </si>
+  <si>
+    <t>Tipo MP,Classe,Durata e Inizio Ciclo Formativo devono essere dei menu a tendina</t>
+  </si>
+  <si>
+    <t>La durata del ciclo cambia in automatico in base al corso</t>
+  </si>
+  <si>
+    <t>Il menu a tendina della classe cambia in automatico in base al corso</t>
+  </si>
+  <si>
+    <t>La fine ciclo formativo cambia in base alla durata del corso e inizio del ciclo</t>
+  </si>
+  <si>
+    <t>È presente anche un campo che indichi il semestre in cui avviene la pianificazione</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutti i dati degli studenti ovvero nome, data di nascita e altre informazioni</t>
   </si>
 </sst>
 </file>
@@ -446,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -511,6 +541,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C168"/>
+  <dimension ref="B1:C184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -879,7 +912,7 @@
     <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -888,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -920,7 +953,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -983,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1015,7 +1048,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1044,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1076,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1162,13 +1195,13 @@
     <row r="56" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
       <c r="C56" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
       <c r="C57" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1179,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1211,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1321,7 +1354,7 @@
         <v>6</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1426,7 +1459,7 @@
         <v>6</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1523,7 +1556,7 @@
     <row r="112" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
       <c r="C112" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1553,7 +1586,7 @@
     <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="5"/>
       <c r="C117" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1606,13 +1639,13 @@
     <row r="125" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="1"/>
       <c r="C125" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
       <c r="C126" s="6" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1678,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1763,7 +1796,7 @@
         <v>6</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1786,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="154" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1794,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1809,8 +1842,8 @@
       <c r="B156" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="4">
-        <v>2</v>
+      <c r="C156" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1830,31 +1863,31 @@
     <row r="159" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B159" s="5"/>
       <c r="C159" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="160" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="5"/>
       <c r="C160" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="5"/>
       <c r="C161" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="162" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="5"/>
       <c r="C162" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="163" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="5"/>
       <c r="C163" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1864,7 +1897,7 @@
     <row r="165" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="7"/>
       <c r="C165" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="166" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1874,15 +1907,109 @@
     <row r="167" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="7"/>
       <c r="C167" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="168" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="7"/>
       <c r="C168" s="24"/>
     </row>
+    <row r="170" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="171" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B173" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B176" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B177" s="5"/>
+      <c r="C177" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B178" s="5"/>
+      <c r="C178" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B179" s="5"/>
+      <c r="C179" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B180" s="5"/>
+      <c r="C180" s="22"/>
+    </row>
+    <row r="181" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B181" s="5"/>
+      <c r="C181" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B182" s="7"/>
+      <c r="C182" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B183" s="7"/>
+      <c r="C183" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B184" s="7"/>
+      <c r="C184" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C179:C180"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="C163:C164"/>

</xml_diff>

<commit_message>
pulizia codice + diari
</commit_message>
<xml_diff>
--- a/Progettazione2/Analisi/requisiti.xlsx
+++ b/Progettazione2/Analisi/requisiti.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MPT\Progettazione2\Analisi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPT\Progettazione2\Analisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Può creare proposte</t>
   </si>
   <si>
-    <t>Aggiunge gli allievi</t>
-  </si>
-  <si>
     <t>Pagina di Log</t>
   </si>
   <si>
@@ -236,18 +233,9 @@
     <t>Creare un manuale che spieghi tutto il funzionamento del sito web</t>
   </si>
   <si>
-    <t>Foglio A4</t>
-  </si>
-  <si>
     <t>Creare un pdf del file che si ha come allegato</t>
   </si>
   <si>
-    <t>Per Bellinzona</t>
-  </si>
-  <si>
-    <t>Aggiungere informazioni del database di SAMB nel sito web</t>
-  </si>
-  <si>
     <t>Informazione classe</t>
   </si>
   <si>
@@ -302,9 +290,6 @@
     <t>REQ-008 progetto precedente</t>
   </si>
   <si>
-    <t>discutere su cosa se si dovesse avere tempo di farlo</t>
-  </si>
-  <si>
     <t>Per ogni log bisogna sapere il docente o l'email che effettua l'azione, il tipo di azione, la pagina in cui avviene l'azione, un ev. descrizione e la data</t>
   </si>
   <si>
@@ -362,10 +347,73 @@
     <t>La fine ciclo formativo cambia in base alla durata del corso e inizio del ciclo</t>
   </si>
   <si>
-    <t>È presente anche un campo che indichi il semestre in cui avviene la pianificazione</t>
-  </si>
-  <si>
-    <t>Bisogna poter vedere tutti i dati degli studenti ovvero nome, data di nascita e altre informazioni</t>
+    <t>importa gli allievi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Può visualizzare gli allievi </t>
+  </si>
+  <si>
+    <t>Può visualizzare il manuale</t>
+  </si>
+  <si>
+    <t>Può visualizzare il foglio degli AIT</t>
+  </si>
+  <si>
+    <t>Progettato in questo progetto</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutti i dati degli studenti ovvero nome, cognome, data di nascita e altre informazioni</t>
+  </si>
+  <si>
+    <t>REQ-012</t>
+  </si>
+  <si>
+    <t>Importazione classe</t>
+  </si>
+  <si>
+    <t>Accessibile solamente all'A</t>
+  </si>
+  <si>
+    <t>L'importazione deve avvenire tramite csv e il file deve essere composto da utente, data di nascita, sezione, altre info PIF e altre info</t>
+  </si>
+  <si>
+    <t>Il manuale deve essere presente sul sito</t>
+  </si>
+  <si>
+    <t>Foglio AIT</t>
+  </si>
+  <si>
+    <t>Il foglio deve essere presente sul sito</t>
+  </si>
+  <si>
+    <t>È presente anche un campo per indicare il semestre in cui avviene la pianificazione</t>
+  </si>
+  <si>
+    <t>REQ-013</t>
+  </si>
+  <si>
+    <t>REQ-014 progetto precedente</t>
+  </si>
+  <si>
+    <t>Pagina Visione pianificazione completa docenti MP</t>
+  </si>
+  <si>
+    <t>REQ-016 progetto precedente</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere tutte le informazioni della pianificazione creata insieme a tutte le parti dei docenti coinvolti, in lettura</t>
+  </si>
+  <si>
+    <t>Bisogna poter vedere le informazioni degli allievi in quella classe</t>
+  </si>
+  <si>
+    <t>Accesso al "Manuale" a tutti quelli loggati</t>
+  </si>
+  <si>
+    <t>Accesso a "Foglio AIT" a tutti quelli loggati</t>
+  </si>
+  <si>
+    <t>REQ-012 progetto precedente</t>
   </si>
 </sst>
 </file>
@@ -392,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,23 +581,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C184"/>
+  <dimension ref="B1:C202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,7 +929,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -912,7 +967,7 @@
     <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -921,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -929,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -953,7 +1008,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -965,744 +1020,747 @@
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="5"/>
-      <c r="C20" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="5"/>
-      <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="5"/>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
+      <c r="B20" s="7"/>
+      <c r="C20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="7"/>
+      <c r="C21" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="5"/>
-      <c r="C23" s="20" t="s">
-        <v>12</v>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="21"/>
-    </row>
-    <row r="25" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8" t="s">
-        <v>13</v>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="7"/>
-      <c r="C27" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="29" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1</v>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="11"/>
+      <c r="C30" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="11"/>
+      <c r="C31" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
+      <c r="B32" s="7"/>
+      <c r="C32" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>87</v>
+      <c r="B33" s="7"/>
+      <c r="C33" s="13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>8</v>
+      <c r="B34" s="7"/>
+      <c r="C34" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="7"/>
-      <c r="C35" s="3" t="s">
-        <v>24</v>
+      <c r="C35" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="7"/>
-      <c r="C36" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="C36" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7"/>
+      <c r="C37" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="38" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="7"/>
+      <c r="C39" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="7"/>
+      <c r="C40" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="7"/>
+      <c r="C41" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="7"/>
+      <c r="C42" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="7"/>
+      <c r="C43" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="7"/>
+      <c r="C44" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="1" t="s">
+      <c r="C46" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C49" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
+    <row r="50" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="1" t="s">
+      <c r="C50" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="9"/>
-      <c r="C44" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="11"/>
-      <c r="C45" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="11"/>
-      <c r="C46" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="7"/>
-      <c r="C47" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="7"/>
-      <c r="C48" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="7"/>
-      <c r="C49" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="7"/>
-      <c r="C50" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="7"/>
-      <c r="C51" s="13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="7"/>
-      <c r="C52" s="13" t="s">
-        <v>36</v>
+      <c r="C52" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
-      <c r="C53" s="13" t="s">
-        <v>37</v>
+      <c r="B53" s="5"/>
+      <c r="C53" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="7"/>
-      <c r="C54" s="13" t="s">
-        <v>38</v>
+      <c r="C54" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="7"/>
-      <c r="C55" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C55" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
-      <c r="C56" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="C56" s="25"/>
     </row>
     <row r="57" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
-      <c r="C57" s="14" t="s">
-        <v>77</v>
+      <c r="C57" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="7"/>
+      <c r="C58" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="15"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="60" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="7"/>
+      <c r="C60" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="7"/>
+      <c r="C61" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="7"/>
+      <c r="C62" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="7"/>
+      <c r="C63" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="7"/>
+      <c r="C64" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="7"/>
+      <c r="C65" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="16"/>
+      <c r="C66" s="15"/>
+    </row>
+    <row r="67" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="1" t="s">
+      <c r="C67" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="1" t="s">
+      <c r="C69" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C70" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="1" t="s">
+    <row r="71" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="1" t="s">
+      <c r="C71" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="7"/>
-      <c r="C66" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="5"/>
-      <c r="C67" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="7"/>
-      <c r="C68" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="7"/>
-      <c r="C69" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="7"/>
-      <c r="C70" s="22"/>
-    </row>
-    <row r="71" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="7"/>
-      <c r="C71" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="7"/>
-      <c r="C72" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
       <c r="C73" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="7"/>
       <c r="C74" s="3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="7"/>
-      <c r="C75" s="14" t="s">
-        <v>60</v>
+      <c r="C75" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="16"/>
-      <c r="C76" s="15"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="77" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>40</v>
+      <c r="B77" s="7"/>
+      <c r="C77" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B78" s="7"/>
       <c r="C78" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="3">
-        <v>1</v>
+      <c r="B79" s="7"/>
+      <c r="C79" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80" s="4">
-        <v>2</v>
+      <c r="B80" s="7"/>
+      <c r="C80" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>90</v>
+      <c r="B81" s="7"/>
+      <c r="C81" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>8</v>
+      <c r="B82" s="7"/>
+      <c r="C82" s="18" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B83" s="7"/>
-      <c r="C83" s="3" t="s">
-        <v>51</v>
+      <c r="C83" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="7"/>
-      <c r="C84" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="7"/>
-      <c r="C85" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
+      <c r="B84" s="5"/>
+      <c r="C84" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="86" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="17"/>
-      <c r="C86" s="13" t="s">
-        <v>53</v>
+      <c r="B86" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="7"/>
+      <c r="B87" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C87" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="5"/>
+      <c r="C92" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="5"/>
+      <c r="C93" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="5"/>
+      <c r="C94" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="5"/>
+      <c r="C95" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="7"/>
-      <c r="C88" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="7"/>
-      <c r="C89" s="3" t="s">
+    <row r="96" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="7"/>
+      <c r="C96" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="7"/>
-      <c r="C90" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="5"/>
-      <c r="C91" s="18" t="s">
+    <row r="97" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="7"/>
+      <c r="C97" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C92" s="15"/>
-    </row>
-    <row r="93" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="1" t="s">
+    <row r="98" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="5"/>
+      <c r="C98" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="100" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="94" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="1" t="s">
+    <row r="101" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C95" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="1" t="s">
+      <c r="C102" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C103" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="1" t="s">
+    <row r="104" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="1" t="s">
+      <c r="C104" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="5"/>
-      <c r="C99" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="5"/>
-      <c r="C100" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="5"/>
-      <c r="C101" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="5"/>
-      <c r="C102" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="7"/>
-      <c r="C103" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="5"/>
-      <c r="C104" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="106" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="5"/>
+      <c r="C106" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="5"/>
+      <c r="C107" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B108" s="5"/>
+      <c r="C108" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="5"/>
+      <c r="C109" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B110" s="7"/>
+      <c r="C110" s="26"/>
+    </row>
+    <row r="111" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="7"/>
+      <c r="C111" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="7"/>
+      <c r="C112" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="7"/>
+      <c r="C113" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="115" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B115" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="1" t="s">
+    <row r="116" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="1" t="s">
+      <c r="C117" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110" s="3"/>
-    </row>
-    <row r="111" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="5"/>
-      <c r="C112" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="5"/>
-      <c r="C113" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="5"/>
-      <c r="C114" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="5"/>
-      <c r="C115" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B116" s="7"/>
-      <c r="C116" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B117" s="5"/>
-      <c r="C117" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="119" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B120" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C121" s="3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="5"/>
+      <c r="C121" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>5</v>
+      <c r="B122" s="5"/>
+      <c r="C122" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="123" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C123" s="3"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="124" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>8</v>
+      <c r="B124" s="5"/>
+      <c r="C124" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B125" s="1"/>
-      <c r="C125" s="19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B125" s="7"/>
+      <c r="C125" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="5"/>
-      <c r="C126" s="6" t="s">
-        <v>113</v>
+      <c r="C126" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="128" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="5"/>
-      <c r="C128" s="6"/>
+      <c r="B128" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="129" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B129" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>68</v>
+        <v>3</v>
+      </c>
+      <c r="C130" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B131" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C131" s="3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B132" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="133" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C133" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="134" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="1"/>
+      <c r="C134" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="5"/>
       <c r="C135" s="6" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="136" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1711,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
     </row>
     <row r="138" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1727,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1742,7 +1800,9 @@
       <c r="B141" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C141" s="3"/>
+      <c r="C141" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="142" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="1" t="s">
@@ -1753,268 +1813,401 @@
       </c>
     </row>
     <row r="143" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B143" s="5"/>
-      <c r="C143" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
+      <c r="B143" s="1"/>
+      <c r="C143" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="5"/>
+      <c r="C144" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="146" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>72</v>
+        <v>0</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="147" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B147" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C147" s="3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="148" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B148" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C148" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>92</v>
+        <v>4</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="5"/>
-      <c r="C151" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="152" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="152" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="1"/>
+      <c r="C152" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="153" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B153" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="154" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
+      <c r="B153" s="5"/>
+      <c r="C153" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="155" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B155" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C155" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="156" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>103</v>
+        <v>1</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="157" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C157" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C157" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="158" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="5"/>
-      <c r="C159" s="6" t="s">
+    <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="1"/>
+      <c r="C161" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="5"/>
+      <c r="C162" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="164" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B166" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B167" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B168" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B169" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B170" s="5"/>
+      <c r="C170" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="5"/>
+      <c r="C171" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="5"/>
+      <c r="C172" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B173" s="5"/>
+      <c r="C173" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="5"/>
+      <c r="C174" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="7"/>
+      <c r="C175" s="25"/>
+    </row>
+    <row r="176" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B176" s="7"/>
+      <c r="C176" s="24" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="160" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="5"/>
-      <c r="C160" s="6" t="s">
+    <row r="177" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B177" s="7"/>
+      <c r="C177" s="25"/>
+    </row>
+    <row r="178" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B178" s="7"/>
+      <c r="C178" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="161" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="5"/>
-      <c r="C161" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="162" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="5"/>
-      <c r="C162" s="8" t="s">
+    <row r="179" spans="2:3" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="180" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B180" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B181" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B182" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B183" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B184" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B185" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B186" s="5"/>
+      <c r="C186" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B187" s="5"/>
+      <c r="C187" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B188" s="5"/>
+      <c r="C188" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B189" s="5"/>
+      <c r="C189" s="25"/>
+    </row>
+    <row r="190" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B190" s="5"/>
+      <c r="C190" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B191" s="7"/>
+      <c r="C191" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B192" s="7"/>
+      <c r="C192" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B193" s="7"/>
+      <c r="C193" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="195" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C195" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="163" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B163" s="5"/>
-      <c r="C163" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="164" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B164" s="7"/>
-      <c r="C164" s="22"/>
-    </row>
-    <row r="165" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B165" s="7"/>
-      <c r="C165" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="166" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B166" s="7"/>
-      <c r="C166" s="22"/>
-    </row>
-    <row r="167" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B167" s="7"/>
-      <c r="C167" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="168" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B168" s="7"/>
-      <c r="C168" s="24"/>
-    </row>
-    <row r="170" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="171" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B171" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="172" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B172" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="173" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B173" s="1" t="s">
+    <row r="196" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B196" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B197" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B174" s="1" t="s">
+      <c r="C197" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B198" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C174" s="4" t="s">
+      <c r="C198" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B175" s="1" t="s">
+    <row r="199" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B199" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C175" s="3"/>
-    </row>
-    <row r="176" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B176" s="1" t="s">
+      <c r="C199" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B200" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="2:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B177" s="5"/>
-      <c r="C177" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="178" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B178" s="5"/>
-      <c r="C178" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="179" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B179" s="5"/>
-      <c r="C179" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="180" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B180" s="5"/>
-      <c r="C180" s="22"/>
-    </row>
-    <row r="181" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B181" s="5"/>
-      <c r="C181" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="182" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B182" s="7"/>
-      <c r="C182" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="183" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B183" s="7"/>
-      <c r="C183" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="184" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B184" s="7"/>
-      <c r="C184" s="25" t="s">
-        <v>112</v>
+    <row r="201" spans="2:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B201" s="5"/>
+      <c r="C201" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B202" s="22"/>
+      <c r="C202" s="20" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C179:C180"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C163:C164"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="C167:C168"/>
+  <mergeCells count="5">
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C109:C110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>